<commit_message>
resolver errores marcas en editar tipo, iddel telefono con conflicto con los selects de agregar equipo y otros
</commit_message>
<xml_diff>
--- a/formato-para_importar_datos.xlsx
+++ b/formato-para_importar_datos.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Equipo" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Modelo" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Unidad" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Equipo" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Modelo" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Unidad" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t xml:space="preserve">Codigo inventario</t>
   </si>
@@ -66,16 +66,10 @@
     <t xml:space="preserve">proveedor</t>
   </si>
   <si>
-    <t xml:space="preserve">123M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">forzado</t>
+    <t xml:space="preserve">fecha_inicio_compra</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id_orden_compra</t>
   </si>
   <si>
     <t xml:space="preserve">NombreModelo</t>
@@ -100,30 +94,6 @@
   </si>
   <si>
     <t xml:space="preserve">Modalidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">u_de_excel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">123_calle_falsa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">concepcion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clasico</t>
-  </si>
-  <si>
-    <t xml:space="preserve">u_de_excel2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">san pedro de la paz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">coronel</t>
   </si>
 </sst>
 </file>
@@ -212,7 +182,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -228,15 +198,121 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="P2" activeCellId="0" sqref="P2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -284,41 +360,27 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="n">
-        <v>583</v>
-      </c>
-      <c r="C2" s="2" t="n">
-        <v>758</v>
-      </c>
-      <c r="G2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="L2" s="3" t="n">
-        <v>45464</v>
-      </c>
-      <c r="M2" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="N2" s="0" t="s">
-        <v>17</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="2"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -346,13 +408,13 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -374,7 +436,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -384,98 +446,52 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>31</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="2"/>
-      <c r="D5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>30</v>
-      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>